<commit_message>
Got everything hooked up to the point where all the data can be loaded off the DB at demand, although it is currently mostly turned off with only one PM being used for initial testing (See the commenting out of the PackageManager enums in PairCollector.kt). Profiling of the time it takes to do this puts it at about 90 minutes to collect the data needed without any concurrency. Working on ProcessPairNew.kt - so far have described what the type of update it is. Still need to quantify the lag involved, and then do something meaningful with these classifications.
</commit_message>
<xml_diff>
--- a/data/ProjectPairsIncludedByPM.xlsx
+++ b/data/ProjectPairsIncludedByPM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\MasseyReadings\Masters\masters\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA00381-F982-48E6-9B40-4B81065E1D77}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461C2D5E-0C20-4F79-8F7E-E99ECADECCDC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{40C7EACB-2B34-480D-9586-89DA186ECD23}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{40C7EACB-2B34-480D-9586-89DA186ECD23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,6 +896,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>SUM(B2:B18)</f>
+        <v>590933</v>
+      </c>
       <c r="F19">
         <f>SUM(F2:F18)</f>
         <v>4273808</v>

</xml_diff>